<commit_message>
Finished loading parts into databse via rake function
</commit_message>
<xml_diff>
--- a/doc/Power Supply List.xlsx
+++ b/doc/Power Supply List.xlsx
@@ -12,12 +12,11 @@
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="125725"/>
-  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="376" uniqueCount="170">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="374" uniqueCount="170">
   <si>
     <t>Power Supplies</t>
   </si>
@@ -115,9 +114,6 @@
     <t> ATX 12V V2.3 /  EPS 12V V2.92</t>
   </si>
   <si>
-    <t>Width (mm)</t>
-  </si>
-  <si>
     <t>http://www.coolermaster-usa.com/product.php?product_id=2998</t>
   </si>
   <si>
@@ -527,6 +523,9 @@
   </si>
   <si>
     <t>ZP-380B</t>
+  </si>
+  <si>
+    <t>Length (mm)</t>
   </si>
 </sst>
 </file>
@@ -881,10 +880,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:V45"/>
+  <dimension ref="A1:V44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="J49" sqref="J49"/>
+    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
+      <selection activeCell="A45" sqref="A45:XFD45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -982,7 +981,7 @@
         <v>16</v>
       </c>
       <c r="V3" t="s">
-        <v>32</v>
+        <v>169</v>
       </c>
     </row>
     <row r="4" spans="1:22">
@@ -1061,16 +1060,16 @@
         <v>18</v>
       </c>
       <c r="C5" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="D5" t="s">
         <v>33</v>
-      </c>
-      <c r="D5" t="s">
-        <v>34</v>
       </c>
       <c r="E5">
         <v>210</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="G5" t="s">
         <v>21</v>
@@ -1129,16 +1128,16 @@
         <v>18</v>
       </c>
       <c r="C6" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="D6" t="s">
         <v>37</v>
-      </c>
-      <c r="D6" t="s">
-        <v>38</v>
       </c>
       <c r="E6">
         <v>160</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="G6" t="s">
         <v>21</v>
@@ -1197,19 +1196,19 @@
         <v>18</v>
       </c>
       <c r="C7" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="D7" s="1" t="s">
         <v>40</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>41</v>
       </c>
       <c r="E7">
         <v>120</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="G7" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="H7">
         <v>135</v>
@@ -1227,10 +1226,10 @@
         <v>5</v>
       </c>
       <c r="M7" t="s">
+        <v>42</v>
+      </c>
+      <c r="N7" s="2" t="s">
         <v>43</v>
-      </c>
-      <c r="N7" s="2" t="s">
-        <v>44</v>
       </c>
       <c r="O7">
         <v>600</v>
@@ -1265,19 +1264,19 @@
         <v>18</v>
       </c>
       <c r="C8" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="D8" s="1" t="s">
         <v>46</v>
-      </c>
-      <c r="D8" s="1" t="s">
-        <v>47</v>
       </c>
       <c r="E8">
         <v>135</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="G8" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="H8">
         <v>135</v>
@@ -1295,10 +1294,10 @@
         <v>5</v>
       </c>
       <c r="M8" t="s">
+        <v>42</v>
+      </c>
+      <c r="N8" s="2" t="s">
         <v>43</v>
-      </c>
-      <c r="N8" s="2" t="s">
-        <v>44</v>
       </c>
       <c r="O8">
         <v>700</v>
@@ -1333,19 +1332,19 @@
         <v>18</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="E9">
         <v>140</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="G9" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="H9">
         <v>135</v>
@@ -1363,7 +1362,7 @@
         <v>6</v>
       </c>
       <c r="M9" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="N9" s="2" t="s">
         <v>31</v>
@@ -1401,19 +1400,19 @@
         <v>18</v>
       </c>
       <c r="C10" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="D10" t="s">
         <v>52</v>
-      </c>
-      <c r="D10" t="s">
-        <v>53</v>
       </c>
       <c r="E10">
         <v>100</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="G10" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="H10">
         <v>120</v>
@@ -1431,7 +1430,7 @@
         <v>3</v>
       </c>
       <c r="M10" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="N10" s="2" t="s">
         <v>30</v>
@@ -1469,19 +1468,19 @@
         <v>18</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E11">
         <v>80</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G11" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="H11">
         <v>120</v>
@@ -1499,7 +1498,7 @@
         <v>3</v>
       </c>
       <c r="M11" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="N11" s="2" t="s">
         <v>30</v>
@@ -1537,19 +1536,19 @@
         <v>18</v>
       </c>
       <c r="C12" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="D12" s="1" t="s">
         <v>60</v>
-      </c>
-      <c r="D12" s="1" t="s">
-        <v>61</v>
       </c>
       <c r="E12">
         <v>230</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="G12" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="H12">
         <v>120</v>
@@ -1567,7 +1566,7 @@
         <v>5</v>
       </c>
       <c r="M12" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="N12" s="2" t="s">
         <v>31</v>
@@ -1605,19 +1604,19 @@
         <v>18</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E13">
         <v>185</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="G13" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="H13">
         <v>120</v>
@@ -1635,7 +1634,7 @@
         <v>5</v>
       </c>
       <c r="M13" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="N13" s="2" t="s">
         <v>31</v>
@@ -1673,19 +1672,19 @@
         <v>18</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D14" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E14">
         <v>60</v>
       </c>
       <c r="F14" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="G14" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="H14">
         <v>120</v>
@@ -1703,7 +1702,7 @@
         <v>3</v>
       </c>
       <c r="M14" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="N14" s="2" t="s">
         <v>30</v>
@@ -1741,19 +1740,19 @@
         <v>18</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D15" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E15">
         <v>80</v>
       </c>
       <c r="F15" s="2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="G15" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="H15">
         <v>120</v>
@@ -1771,7 +1770,7 @@
         <v>3</v>
       </c>
       <c r="M15" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="N15" s="2" t="s">
         <v>30</v>
@@ -1809,19 +1808,19 @@
         <v>18</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D16" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="E16">
         <v>70</v>
       </c>
       <c r="F16" s="2" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="G16" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="H16">
         <v>120</v>
@@ -1839,7 +1838,7 @@
         <v>3</v>
       </c>
       <c r="M16" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="N16" s="2" t="s">
         <v>30</v>
@@ -1877,19 +1876,19 @@
         <v>18</v>
       </c>
       <c r="C17" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="D17" t="s">
         <v>78</v>
-      </c>
-      <c r="D17" t="s">
-        <v>79</v>
       </c>
       <c r="E17">
         <v>50</v>
       </c>
       <c r="F17" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="G17" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="H17">
         <v>80</v>
@@ -1901,13 +1900,13 @@
         <v>3</v>
       </c>
       <c r="K17" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="L17">
         <v>5</v>
       </c>
       <c r="M17" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="N17" s="2" t="s">
         <v>30</v>
@@ -1945,19 +1944,19 @@
         <v>18</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D18" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E18">
         <v>30</v>
       </c>
       <c r="F18" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="G18" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="H18">
         <v>120</v>
@@ -1969,13 +1968,13 @@
         <v>3</v>
       </c>
       <c r="K18" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="L18">
         <v>3</v>
       </c>
       <c r="M18" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="N18" s="2" t="s">
         <v>30</v>
@@ -2013,19 +2012,19 @@
         <v>18</v>
       </c>
       <c r="C19" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="D19" t="s">
         <v>84</v>
-      </c>
-      <c r="D19" t="s">
-        <v>85</v>
       </c>
       <c r="E19">
         <v>35</v>
       </c>
       <c r="F19" s="2" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="G19" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="H19">
         <v>120</v>
@@ -2037,13 +2036,13 @@
         <v>4</v>
       </c>
       <c r="K19" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="L19">
         <v>3</v>
       </c>
       <c r="M19" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="N19" s="2" t="s">
         <v>30</v>
@@ -2081,19 +2080,19 @@
         <v>18</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D20" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="E20">
         <v>40</v>
       </c>
       <c r="F20" s="2" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="G20" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="H20">
         <v>120</v>
@@ -2105,13 +2104,13 @@
         <v>4</v>
       </c>
       <c r="K20" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="L20">
         <v>3</v>
       </c>
       <c r="M20" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="N20" s="2" t="s">
         <v>30</v>
@@ -2146,22 +2145,22 @@
         <v>17</v>
       </c>
       <c r="B22" t="s">
+        <v>90</v>
+      </c>
+      <c r="C22" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="C22" s="1" t="s">
+      <c r="D22" t="s">
         <v>92</v>
-      </c>
-      <c r="D22" t="s">
-        <v>93</v>
       </c>
       <c r="E22">
         <v>155</v>
       </c>
       <c r="F22" t="s">
+        <v>93</v>
+      </c>
+      <c r="G22" t="s">
         <v>94</v>
-      </c>
-      <c r="G22" t="s">
-        <v>95</v>
       </c>
       <c r="H22">
         <v>140</v>
@@ -2214,22 +2213,22 @@
         <v>17</v>
       </c>
       <c r="B23" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C23" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="D23" t="s">
         <v>96</v>
-      </c>
-      <c r="D23" t="s">
-        <v>97</v>
       </c>
       <c r="E23">
         <v>170</v>
       </c>
       <c r="F23" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="G23" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="H23">
         <v>140</v>
@@ -2282,22 +2281,22 @@
         <v>17</v>
       </c>
       <c r="B24" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C24" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="D24" t="s">
         <v>99</v>
-      </c>
-      <c r="D24" t="s">
-        <v>100</v>
       </c>
       <c r="E24">
         <v>110</v>
       </c>
       <c r="F24" t="s">
+        <v>100</v>
+      </c>
+      <c r="G24" t="s">
         <v>101</v>
-      </c>
-      <c r="G24" t="s">
-        <v>102</v>
       </c>
       <c r="H24">
         <v>140</v>
@@ -2315,10 +2314,10 @@
         <v>6</v>
       </c>
       <c r="M24" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="N24" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="O24">
         <v>575</v>
@@ -2350,22 +2349,22 @@
         <v>17</v>
       </c>
       <c r="B25" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C25" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="D25" t="s">
         <v>104</v>
-      </c>
-      <c r="D25" t="s">
-        <v>105</v>
       </c>
       <c r="E25">
         <v>125</v>
       </c>
       <c r="F25" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="G25" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="H25">
         <v>140</v>
@@ -2383,10 +2382,10 @@
         <v>6</v>
       </c>
       <c r="M25" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="N25" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="O25">
         <v>675</v>
@@ -2418,22 +2417,22 @@
         <v>17</v>
       </c>
       <c r="B26" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C26" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="D26" t="s">
         <v>107</v>
-      </c>
-      <c r="D26" t="s">
-        <v>108</v>
       </c>
       <c r="E26">
         <v>140</v>
       </c>
       <c r="F26" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="G26" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="H26">
         <v>140</v>
@@ -2451,10 +2450,10 @@
         <v>6</v>
       </c>
       <c r="M26" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="N26" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="O26">
         <v>775</v>
@@ -2486,22 +2485,22 @@
         <v>17</v>
       </c>
       <c r="B27" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C27" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="D27" t="s">
         <v>110</v>
-      </c>
-      <c r="D27" t="s">
-        <v>111</v>
       </c>
       <c r="E27">
         <v>160</v>
       </c>
       <c r="F27" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="G27" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="H27">
         <v>140</v>
@@ -2519,10 +2518,10 @@
         <v>6</v>
       </c>
       <c r="M27" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="N27" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="O27">
         <v>875</v>
@@ -2554,22 +2553,22 @@
         <v>17</v>
       </c>
       <c r="B28" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C28" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="D28" t="s">
         <v>112</v>
-      </c>
-      <c r="D28" t="s">
-        <v>113</v>
       </c>
       <c r="E28">
         <v>100</v>
       </c>
       <c r="F28" t="s">
+        <v>113</v>
+      </c>
+      <c r="G28" t="s">
         <v>114</v>
-      </c>
-      <c r="G28" t="s">
-        <v>115</v>
       </c>
       <c r="H28">
         <v>120</v>
@@ -2587,7 +2586,7 @@
         <v>6</v>
       </c>
       <c r="M28" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="N28" s="2" t="s">
         <v>30</v>
@@ -2622,22 +2621,22 @@
         <v>17</v>
       </c>
       <c r="B29" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C29" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="D29" t="s">
         <v>116</v>
-      </c>
-      <c r="D29" t="s">
-        <v>117</v>
       </c>
       <c r="E29">
         <v>110</v>
       </c>
       <c r="F29" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="G29" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="H29">
         <v>120</v>
@@ -2655,7 +2654,7 @@
         <v>6</v>
       </c>
       <c r="M29" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="N29" s="2" t="s">
         <v>30</v>
@@ -2690,22 +2689,22 @@
         <v>17</v>
       </c>
       <c r="B30" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C30" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="D30" t="s">
         <v>119</v>
-      </c>
-      <c r="D30" t="s">
-        <v>120</v>
       </c>
       <c r="E30">
         <v>75</v>
       </c>
       <c r="F30" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="G30" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="H30">
         <v>120</v>
@@ -2717,16 +2716,16 @@
         <v>4</v>
       </c>
       <c r="K30" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="L30">
         <v>8</v>
       </c>
       <c r="M30" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="N30" s="2" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="O30">
         <v>600</v>
@@ -2758,22 +2757,22 @@
         <v>17</v>
       </c>
       <c r="B31" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C31" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="D31" t="s">
         <v>124</v>
-      </c>
-      <c r="D31" t="s">
-        <v>125</v>
       </c>
       <c r="E31">
         <v>100</v>
       </c>
       <c r="F31" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="G31" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="H31">
         <v>140</v>
@@ -2791,10 +2790,10 @@
         <v>6</v>
       </c>
       <c r="M31" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="N31" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="O31">
         <v>550</v>
@@ -2826,22 +2825,22 @@
         <v>17</v>
       </c>
       <c r="B32" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C32" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="D32" t="s">
         <v>127</v>
-      </c>
-      <c r="D32" t="s">
-        <v>128</v>
       </c>
       <c r="E32">
         <v>130</v>
       </c>
       <c r="F32" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="G32" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="H32">
         <v>140</v>
@@ -2859,10 +2858,10 @@
         <v>6</v>
       </c>
       <c r="M32" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="N32" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="O32">
         <v>750</v>
@@ -2894,22 +2893,22 @@
         <v>17</v>
       </c>
       <c r="B33" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C33" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="D33" t="s">
         <v>131</v>
-      </c>
-      <c r="D33" t="s">
-        <v>132</v>
       </c>
       <c r="E33">
         <v>200</v>
       </c>
       <c r="F33" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="G33" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="H33">
         <v>140</v>
@@ -2927,10 +2926,10 @@
         <v>8</v>
       </c>
       <c r="M33" t="s">
+        <v>42</v>
+      </c>
+      <c r="N33" s="2" t="s">
         <v>43</v>
-      </c>
-      <c r="N33" s="2" t="s">
-        <v>44</v>
       </c>
       <c r="O33">
         <v>1200</v>
@@ -2962,22 +2961,22 @@
         <v>17</v>
       </c>
       <c r="B34" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C34" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="D34" t="s">
         <v>135</v>
-      </c>
-      <c r="D34" t="s">
-        <v>136</v>
       </c>
       <c r="E34">
         <v>185</v>
       </c>
       <c r="F34" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="G34" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="H34">
         <v>140</v>
@@ -2995,10 +2994,10 @@
         <v>8</v>
       </c>
       <c r="M34" t="s">
+        <v>42</v>
+      </c>
+      <c r="N34" s="2" t="s">
         <v>43</v>
-      </c>
-      <c r="N34" s="2" t="s">
-        <v>44</v>
       </c>
       <c r="O34">
         <v>1000</v>
@@ -3030,22 +3029,22 @@
         <v>17</v>
       </c>
       <c r="B35" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C35" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="D35" t="s">
         <v>137</v>
-      </c>
-      <c r="D35" t="s">
-        <v>138</v>
       </c>
       <c r="E35">
         <v>135</v>
       </c>
       <c r="F35" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="G35" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="H35">
         <v>140</v>
@@ -3063,10 +3062,10 @@
         <v>7</v>
       </c>
       <c r="M35" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="N35" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="O35">
         <v>850</v>
@@ -3098,22 +3097,22 @@
         <v>17</v>
       </c>
       <c r="B36" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C36" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="D36" t="s">
         <v>141</v>
-      </c>
-      <c r="D36" t="s">
-        <v>142</v>
       </c>
       <c r="E36">
         <v>110</v>
       </c>
       <c r="F36" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="G36" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="H36">
         <v>140</v>
@@ -3131,10 +3130,10 @@
         <v>7</v>
       </c>
       <c r="M36" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="N36" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="O36">
         <v>750</v>
@@ -3166,22 +3165,22 @@
         <v>17</v>
       </c>
       <c r="B37" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C37" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="D37" t="s">
         <v>144</v>
-      </c>
-      <c r="D37" t="s">
-        <v>145</v>
       </c>
       <c r="E37">
         <v>90</v>
       </c>
       <c r="F37" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="G37" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="H37">
         <v>140</v>
@@ -3199,10 +3198,10 @@
         <v>6</v>
       </c>
       <c r="M37" t="s">
+        <v>42</v>
+      </c>
+      <c r="N37" s="2" t="s">
         <v>43</v>
-      </c>
-      <c r="N37" s="2" t="s">
-        <v>44</v>
       </c>
       <c r="O37">
         <v>650</v>
@@ -3234,22 +3233,22 @@
         <v>17</v>
       </c>
       <c r="B39" t="s">
+        <v>146</v>
+      </c>
+      <c r="C39" s="1" t="s">
         <v>147</v>
       </c>
-      <c r="C39" s="1" t="s">
+      <c r="D39" t="s">
         <v>148</v>
-      </c>
-      <c r="D39" t="s">
-        <v>149</v>
       </c>
       <c r="E39">
         <v>105</v>
       </c>
       <c r="F39" t="s">
+        <v>149</v>
+      </c>
+      <c r="G39" t="s">
         <v>150</v>
-      </c>
-      <c r="G39" t="s">
-        <v>151</v>
       </c>
       <c r="H39">
         <v>140</v>
@@ -3267,10 +3266,10 @@
         <v>6</v>
       </c>
       <c r="M39" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="N39" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="O39">
         <v>750</v>
@@ -3302,22 +3301,22 @@
         <v>17</v>
       </c>
       <c r="B40" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="C40" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="D40" t="s">
         <v>152</v>
-      </c>
-      <c r="D40" t="s">
-        <v>153</v>
       </c>
       <c r="E40">
         <v>210</v>
       </c>
       <c r="F40" t="s">
+        <v>153</v>
+      </c>
+      <c r="G40" t="s">
         <v>154</v>
-      </c>
-      <c r="G40" t="s">
-        <v>155</v>
       </c>
       <c r="H40">
         <v>140</v>
@@ -3335,10 +3334,10 @@
         <v>9</v>
       </c>
       <c r="M40" t="s">
+        <v>42</v>
+      </c>
+      <c r="N40" s="2" t="s">
         <v>43</v>
-      </c>
-      <c r="N40" s="2" t="s">
-        <v>44</v>
       </c>
       <c r="O40">
         <v>1200</v>
@@ -3370,22 +3369,22 @@
         <v>17</v>
       </c>
       <c r="B41" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="C41" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="D41" s="1" t="s">
         <v>157</v>
-      </c>
-      <c r="D41" s="1" t="s">
-        <v>158</v>
       </c>
       <c r="E41">
         <v>110</v>
       </c>
       <c r="F41" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="G41" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="H41">
         <v>140</v>
@@ -3403,10 +3402,10 @@
         <v>8</v>
       </c>
       <c r="M41" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="N41" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="O41">
         <v>950</v>
@@ -3438,22 +3437,22 @@
         <v>17</v>
       </c>
       <c r="B42" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="C42" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="D42" t="s">
         <v>159</v>
-      </c>
-      <c r="D42" t="s">
-        <v>160</v>
       </c>
       <c r="E42">
         <v>50</v>
       </c>
       <c r="F42" t="s">
+        <v>160</v>
+      </c>
+      <c r="G42" t="s">
         <v>161</v>
-      </c>
-      <c r="G42" t="s">
-        <v>162</v>
       </c>
       <c r="H42">
         <v>140</v>
@@ -3465,16 +3464,16 @@
         <v>4</v>
       </c>
       <c r="K42" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="L42">
         <v>4</v>
       </c>
       <c r="M42" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="N42" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="O42">
         <v>550</v>
@@ -3506,22 +3505,22 @@
         <v>17</v>
       </c>
       <c r="B43" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="C43" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="D43" s="1" t="s">
         <v>164</v>
-      </c>
-      <c r="D43" s="1" t="s">
-        <v>165</v>
       </c>
       <c r="E43">
         <v>45</v>
       </c>
       <c r="F43" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="G43" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="H43">
         <v>140</v>
@@ -3533,16 +3532,16 @@
         <v>2</v>
       </c>
       <c r="K43" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="L43">
         <v>6</v>
       </c>
       <c r="M43" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="N43" s="2" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="O43">
         <v>600</v>
@@ -3574,22 +3573,22 @@
         <v>17</v>
       </c>
       <c r="B44" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="D44" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="E44">
         <v>55</v>
       </c>
       <c r="F44" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="G44" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="H44">
         <v>120</v>
@@ -3601,16 +3600,16 @@
         <v>4</v>
       </c>
       <c r="K44" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="L44">
         <v>6</v>
       </c>
       <c r="M44" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="N44" s="2" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="O44">
         <v>380</v>
@@ -3635,14 +3634,6 @@
       </c>
       <c r="V44">
         <v>142</v>
-      </c>
-    </row>
-    <row r="45" spans="1:22">
-      <c r="A45" t="s">
-        <v>17</v>
-      </c>
-      <c r="B45" t="s">
-        <v>147</v>
       </c>
     </row>
   </sheetData>

</xml_diff>